<commit_message>
update figs under PS
</commit_message>
<xml_diff>
--- a/outcome/appendix/Supplementary Appendix 2.xlsx
+++ b/outcome/appendix/Supplementary Appendix 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stuxmueducn-my.sharepoint.com/personal/kanggle_stu_xmu_edu_cn/Documents/XMU/likangguo/2022/11 COVID_impact_luoli/code_PHSM/outcome/appendix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_83355CB94646B645A825410C301FFDC09747C93D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3813C44-6539-4B26-8AE3-9F86F6445231}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_83355CB94646B645A825410C301FFDC09747C93D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77879326-1399-447A-A448-A1376FD3144A}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,6 +383,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -47958,6 +47962,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="22.75" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">

</xml_diff>